<commit_message>
modify raw.xlsx and remove the space char in XiaoTian_rule.txt
</commit_message>
<xml_diff>
--- a/raw.xlsx
+++ b/raw.xlsx
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="131">
   <si>
     <t>Test Items</t>
   </si>
@@ -414,103 +414,19 @@
     <t>Lite_BM</t>
   </si>
   <si>
-    <t>Aruba_HS</t>
-  </si>
-  <si>
-    <t>Aruba_FS</t>
-  </si>
-  <si>
-    <t>TWR-K64</t>
-  </si>
-  <si>
-    <t>FRDM-K82</t>
-  </si>
-  <si>
-    <t>FRDM-KL81</t>
-  </si>
-  <si>
-    <t>FRDM-KL82</t>
-  </si>
-  <si>
-    <t>Aruba</t>
-  </si>
-  <si>
-    <t>TWR-K65</t>
-  </si>
-  <si>
-    <t>FRDM-K66</t>
-  </si>
-  <si>
-    <t>TWR-K80</t>
-  </si>
-  <si>
-    <t>TWR-KL81</t>
-  </si>
-  <si>
-    <t>TWR-KL82</t>
-  </si>
-  <si>
-    <t>TWR-K81</t>
-  </si>
-  <si>
-    <t>FRDM-K28_HS</t>
-  </si>
-  <si>
-    <t>Aruba_S_HS</t>
-  </si>
-  <si>
-    <t>Aruba_S_FS</t>
-  </si>
-  <si>
     <t>FRDM-K28F</t>
   </si>
   <si>
-    <t>FRDM-KL27</t>
-  </si>
-  <si>
-    <t>FRDM-KL28</t>
-  </si>
-  <si>
-    <t>TWR-KL28</t>
-  </si>
-  <si>
-    <t>TWR-K65_HS</t>
-  </si>
-  <si>
     <t>FRDM-K28</t>
   </si>
   <si>
-    <t>FRM-K82</t>
-  </si>
-  <si>
-    <t>FRDM-K28_FS</t>
-  </si>
-  <si>
-    <t>FRDM-K64</t>
-  </si>
-  <si>
-    <t>TWR-K65_FS</t>
-  </si>
-  <si>
-    <t>TWR-K21D50</t>
-  </si>
-  <si>
-    <t>TWR-K60</t>
-  </si>
-  <si>
     <t>MAPS-KS22</t>
   </si>
   <si>
     <t>LPCXPRESS545114</t>
   </si>
   <si>
-    <t>TWR-K21F120</t>
-  </si>
-  <si>
     <t>host_audio_speaker</t>
-  </si>
-  <si>
-    <t>FRDM-KL46</t>
   </si>
   <si>
     <t>BM_Release</t>
@@ -575,6 +491,108 @@
   </si>
   <si>
     <t>KSDK_freertos</t>
+  </si>
+  <si>
+    <t>LPCX-pRESSO54608_HS</t>
+  </si>
+  <si>
+    <t>LPCX-pRESSO54608_FS</t>
+  </si>
+  <si>
+    <t>LPCX-pRESSO54608</t>
+  </si>
+  <si>
+    <t>LPCX-pRESSO54608_S_FS</t>
+  </si>
+  <si>
+    <t>LPCX-pRESSO54S608_HS</t>
+  </si>
+  <si>
+    <t>LPCX-pRESSO54S608_FS</t>
+  </si>
+  <si>
+    <t>LPCX-PRESS545114</t>
+  </si>
+  <si>
+    <t>TWR-K65F180M</t>
+  </si>
+  <si>
+    <t>TWR-K65F180M_HS</t>
+  </si>
+  <si>
+    <t>TWR-K65F180M_FS</t>
+  </si>
+  <si>
+    <t>TWR-K64F120M</t>
+  </si>
+  <si>
+    <t>TWR-K60D100M</t>
+  </si>
+  <si>
+    <t>FRDM-K66F</t>
+  </si>
+  <si>
+    <t>FRDM-K28F_FS</t>
+  </si>
+  <si>
+    <t>FRDM-K28F_HS</t>
+  </si>
+  <si>
+    <t>TWR-K80F150M</t>
+  </si>
+  <si>
+    <t>TWR-K81F150M</t>
+  </si>
+  <si>
+    <t>TWR-K21D50M</t>
+  </si>
+  <si>
+    <t>TWR-K21F120M</t>
+  </si>
+  <si>
+    <t>FRDM-KL27Z</t>
+  </si>
+  <si>
+    <t>FRDM-KL81Z</t>
+  </si>
+  <si>
+    <t>FRDM-KL82Z</t>
+  </si>
+  <si>
+    <t>FRDM-KL28Z</t>
+  </si>
+  <si>
+    <t>FRDM-K64F</t>
+  </si>
+  <si>
+    <t>FRDM-K82F</t>
+  </si>
+  <si>
+    <t>FRDM-KL46Z</t>
+  </si>
+  <si>
+    <t>TWR-KL81F150</t>
+  </si>
+  <si>
+    <t>TWR-KL82Z72M</t>
+  </si>
+  <si>
+    <t>TWR-KL28Z72M</t>
+  </si>
+  <si>
+    <t>TWR-KL81Z72M</t>
+  </si>
+  <si>
+    <t>FRM-K82F</t>
+  </si>
+  <si>
+    <t>IAR</t>
+  </si>
+  <si>
+    <t>APP-USB0-CV_Test_Host</t>
+  </si>
+  <si>
+    <t>APP-USB0-CV_Test_Device</t>
   </si>
 </sst>
 </file>
@@ -809,20 +827,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -830,11 +842,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1151,10 +1169,10 @@
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="18" t="s">
         <v>42</v>
       </c>
@@ -1177,10 +1195,10 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
-        <v>1</v>
-      </c>
-      <c r="B2" s="33" t="s">
+      <c r="A2" s="36">
+        <v>1</v>
+      </c>
+      <c r="B2" s="38" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1188,153 +1206,153 @@
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="39">
+      <c r="F2" s="32">
         <v>4</v>
       </c>
       <c r="G2" s="17"/>
-      <c r="H2" s="38">
+      <c r="H2" s="31">
         <v>4</v>
       </c>
-      <c r="I2" s="39">
+      <c r="I2" s="32">
         <v>4</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="33"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
-      <c r="F3" s="39"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="17"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="39"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="17"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="39"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="39"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="39"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="17"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="39"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="39"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="39"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="39"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="17"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="32"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="39"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="39"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="16"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="39"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="39"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="16"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="32"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="35">
+      <c r="A12" s="36">
         <v>2</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="38" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1342,140 +1360,140 @@
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="39">
+      <c r="F12" s="32">
         <v>10</v>
       </c>
       <c r="G12" s="16"/>
-      <c r="H12" s="38">
+      <c r="H12" s="31">
         <v>10</v>
       </c>
-      <c r="I12" s="39">
+      <c r="I12" s="32">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="39"/>
+      <c r="F13" s="32"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="39"/>
+      <c r="F14" s="32"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="32"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="39"/>
+      <c r="F15" s="32"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="39"/>
+      <c r="F16" s="32"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="39"/>
+      <c r="F17" s="32"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="39"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="39"/>
+      <c r="F18" s="32"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="32"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="39"/>
+      <c r="F19" s="32"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="39"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="32"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="39"/>
+      <c r="F20" s="32"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="32"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="35"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="39"/>
+      <c r="F21" s="32"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="39"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="32"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="35">
+      <c r="A22" s="36">
         <v>3</v>
       </c>
-      <c r="B22" s="32" t="s">
-        <v>112</v>
+      <c r="B22" s="33" t="s">
+        <v>84</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>11</v>
@@ -1495,14 +1513,14 @@
       <c r="H22" s="10">
         <v>0.25</v>
       </c>
-      <c r="I22" s="39">
+      <c r="I22" s="32">
         <f>SUM(F22:F42)</f>
         <v>9.3000000000000025</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="32"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
@@ -1521,11 +1539,11 @@
       <c r="H23" s="10">
         <v>0.25</v>
       </c>
-      <c r="I23" s="39"/>
+      <c r="I23" s="32"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="32"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
@@ -1544,11 +1562,11 @@
       <c r="H24" s="10">
         <v>0.25</v>
       </c>
-      <c r="I24" s="39"/>
+      <c r="I24" s="32"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="3" t="s">
         <v>9</v>
       </c>
@@ -1567,11 +1585,11 @@
       <c r="H25" s="10">
         <v>0.25</v>
       </c>
-      <c r="I25" s="39"/>
+      <c r="I25" s="32"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="32"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="3" t="s">
         <v>10</v>
       </c>
@@ -1590,11 +1608,11 @@
       <c r="H26" s="10">
         <v>0.25</v>
       </c>
-      <c r="I26" s="39"/>
+      <c r="I26" s="32"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="32"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="3" t="s">
         <v>29</v>
       </c>
@@ -1613,13 +1631,13 @@
       <c r="H27" s="10">
         <v>0.25</v>
       </c>
-      <c r="I27" s="39"/>
+      <c r="I27" s="32"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="32"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="3" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -1630,11 +1648,11 @@
       <c r="H28" s="22">
         <v>0.25</v>
       </c>
-      <c r="I28" s="39"/>
+      <c r="I28" s="32"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="32"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="9" t="s">
         <v>41</v>
       </c>
@@ -1653,11 +1671,11 @@
       <c r="H29" s="11">
         <v>0.2</v>
       </c>
-      <c r="I29" s="39"/>
+      <c r="I29" s="32"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="32"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="2" t="s">
         <v>3</v>
       </c>
@@ -1676,11 +1694,11 @@
       <c r="H30" s="11">
         <v>0.2</v>
       </c>
-      <c r="I30" s="39"/>
+      <c r="I30" s="32"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="32"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="2" t="s">
         <v>4</v>
       </c>
@@ -1699,11 +1717,11 @@
       <c r="H31" s="11">
         <v>0.2</v>
       </c>
-      <c r="I31" s="39"/>
+      <c r="I31" s="32"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
-      <c r="B32" s="32"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="2" t="s">
         <v>5</v>
       </c>
@@ -1722,11 +1740,11 @@
       <c r="H32" s="11">
         <v>0.2</v>
       </c>
-      <c r="I32" s="39"/>
+      <c r="I32" s="32"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
-      <c r="B33" s="32"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="2" t="s">
         <v>7</v>
       </c>
@@ -1745,11 +1763,11 @@
       <c r="H33" s="11">
         <v>0.4</v>
       </c>
-      <c r="I33" s="39"/>
+      <c r="I33" s="32"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
-      <c r="B34" s="32"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="2" t="s">
         <v>12</v>
       </c>
@@ -1768,11 +1786,11 @@
       <c r="H34" s="11">
         <v>0.4</v>
       </c>
-      <c r="I34" s="39"/>
+      <c r="I34" s="32"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
-      <c r="B35" s="32"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="2" t="s">
         <v>13</v>
       </c>
@@ -1791,11 +1809,11 @@
       <c r="H35" s="11">
         <v>0.2</v>
       </c>
-      <c r="I35" s="39"/>
+      <c r="I35" s="32"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="32"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="2" t="s">
         <v>30</v>
       </c>
@@ -1814,11 +1832,11 @@
       <c r="H36" s="11">
         <v>0.2</v>
       </c>
-      <c r="I36" s="39"/>
+      <c r="I36" s="32"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
-      <c r="B37" s="32"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="2" t="s">
         <v>27</v>
       </c>
@@ -1837,11 +1855,11 @@
       <c r="H37" s="11">
         <v>0.2</v>
       </c>
-      <c r="I37" s="39"/>
+      <c r="I37" s="32"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="32"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="2" t="s">
         <v>31</v>
       </c>
@@ -1860,11 +1878,11 @@
       <c r="H38" s="11">
         <v>0.2</v>
       </c>
-      <c r="I38" s="39"/>
+      <c r="I38" s="32"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
-      <c r="B39" s="32"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="6" t="s">
         <v>38</v>
       </c>
@@ -1883,11 +1901,11 @@
       <c r="H39" s="11">
         <v>0.2</v>
       </c>
-      <c r="I39" s="39"/>
+      <c r="I39" s="32"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
-      <c r="B40" s="32"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="33"/>
       <c r="C40" s="6" t="s">
         <v>39</v>
       </c>
@@ -1906,11 +1924,11 @@
       <c r="H40" s="11">
         <v>0.2</v>
       </c>
-      <c r="I40" s="39"/>
+      <c r="I40" s="32"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
-      <c r="B41" s="32"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="33"/>
       <c r="C41" s="6" t="s">
         <v>40</v>
       </c>
@@ -1929,11 +1947,11 @@
       <c r="H41" s="11">
         <v>0.2</v>
       </c>
-      <c r="I41" s="39"/>
+      <c r="I41" s="32"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
-      <c r="B42" s="32"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="33"/>
       <c r="C42" s="2" t="s">
         <v>14</v>
       </c>
@@ -1952,13 +1970,13 @@
       <c r="H42" s="11">
         <v>0.2</v>
       </c>
-      <c r="I42" s="39"/>
+      <c r="I42" s="32"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="35">
+      <c r="A43" s="36">
         <v>4</v>
       </c>
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="38" t="s">
         <v>35</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1979,13 +1997,13 @@
       <c r="H43" s="10">
         <v>1</v>
       </c>
-      <c r="I43" s="39">
+      <c r="I43" s="32">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="38"/>
       <c r="C44" s="2" t="s">
         <v>16</v>
       </c>
@@ -2004,11 +2022,11 @@
       <c r="H44" s="10">
         <v>1</v>
       </c>
-      <c r="I44" s="39"/>
+      <c r="I44" s="32"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="2" t="s">
         <v>17</v>
       </c>
@@ -2027,11 +2045,11 @@
       <c r="H45" s="10">
         <v>1</v>
       </c>
-      <c r="I45" s="39"/>
+      <c r="I45" s="32"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="38"/>
       <c r="C46" s="2" t="s">
         <v>18</v>
       </c>
@@ -2050,13 +2068,13 @@
       <c r="H46" s="10">
         <v>1</v>
       </c>
-      <c r="I46" s="39"/>
+      <c r="I46" s="32"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="35">
+      <c r="A47" s="36">
         <v>5</v>
       </c>
-      <c r="B47" s="33" t="s">
+      <c r="B47" s="38" t="s">
         <v>36</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -2075,14 +2093,14 @@
       <c r="H47" s="10">
         <v>0.15</v>
       </c>
-      <c r="I47" s="39">
+      <c r="I47" s="32">
         <f>SUM(F47:F54)</f>
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
-      <c r="B48" s="33"/>
+      <c r="A48" s="36"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="2" t="s">
         <v>20</v>
       </c>
@@ -2099,11 +2117,11 @@
       <c r="H48" s="10">
         <v>0.1</v>
       </c>
-      <c r="I48" s="39"/>
+      <c r="I48" s="32"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
-      <c r="B49" s="33"/>
+      <c r="A49" s="36"/>
+      <c r="B49" s="38"/>
       <c r="C49" s="2" t="s">
         <v>22</v>
       </c>
@@ -2120,11 +2138,11 @@
       <c r="H49" s="10">
         <v>0.15</v>
       </c>
-      <c r="I49" s="39"/>
+      <c r="I49" s="32"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
-      <c r="B50" s="33"/>
+      <c r="A50" s="36"/>
+      <c r="B50" s="38"/>
       <c r="C50" s="2" t="s">
         <v>21</v>
       </c>
@@ -2141,11 +2159,11 @@
       <c r="H50" s="10">
         <v>0.1</v>
       </c>
-      <c r="I50" s="39"/>
+      <c r="I50" s="32"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
-      <c r="B51" s="33"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="38"/>
       <c r="C51" s="2" t="s">
         <v>23</v>
       </c>
@@ -2162,11 +2180,11 @@
       <c r="H51" s="10">
         <v>0.15</v>
       </c>
-      <c r="I51" s="39"/>
+      <c r="I51" s="32"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
-      <c r="B52" s="33"/>
+      <c r="A52" s="36"/>
+      <c r="B52" s="38"/>
       <c r="C52" s="2" t="s">
         <v>24</v>
       </c>
@@ -2183,11 +2201,11 @@
       <c r="H52" s="10">
         <v>0.1</v>
       </c>
-      <c r="I52" s="39"/>
+      <c r="I52" s="32"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="35"/>
-      <c r="B53" s="33"/>
+      <c r="A53" s="36"/>
+      <c r="B53" s="38"/>
       <c r="C53" s="2" t="s">
         <v>25</v>
       </c>
@@ -2204,11 +2222,11 @@
       <c r="H53" s="10">
         <v>0.15</v>
       </c>
-      <c r="I53" s="39"/>
+      <c r="I53" s="32"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
-      <c r="B54" s="33"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="38"/>
       <c r="C54" s="2" t="s">
         <v>26</v>
       </c>
@@ -2225,16 +2243,16 @@
       <c r="H54" s="10">
         <v>0.1</v>
       </c>
-      <c r="I54" s="39"/>
+      <c r="I54" s="32"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>6</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C55" s="34"/>
+      <c r="C55" s="39"/>
       <c r="F55" s="14">
         <v>0.3</v>
       </c>
@@ -2250,10 +2268,10 @@
       <c r="A56" s="7">
         <v>7</v>
       </c>
-      <c r="B56" s="34" t="s">
+      <c r="B56" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="34"/>
+      <c r="C56" s="39"/>
       <c r="F56" s="14">
         <v>0.5</v>
       </c>
@@ -2269,10 +2287,10 @@
       <c r="A57" s="7">
         <v>8</v>
       </c>
-      <c r="B57" s="34" t="s">
+      <c r="B57" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="34"/>
+      <c r="C57" s="39"/>
       <c r="F57" s="14">
         <v>3</v>
       </c>
@@ -2285,10 +2303,10 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="36">
+      <c r="A58" s="34">
         <v>9</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="33" t="s">
         <v>57</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -2306,14 +2324,14 @@
       <c r="H58" s="8">
         <v>0.1</v>
       </c>
-      <c r="I58" s="39">
+      <c r="I58" s="32">
         <f>SUM(F58:F71)</f>
         <v>1.0500000000000003</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="37"/>
-      <c r="B59" s="32"/>
+      <c r="A59" s="35"/>
+      <c r="B59" s="33"/>
       <c r="C59" s="3" t="s">
         <v>8</v>
       </c>
@@ -2329,11 +2347,11 @@
       <c r="H59" s="8">
         <v>0.1</v>
       </c>
-      <c r="I59" s="39"/>
+      <c r="I59" s="32"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="37"/>
-      <c r="B60" s="32"/>
+      <c r="A60" s="35"/>
+      <c r="B60" s="33"/>
       <c r="C60" s="3" t="s">
         <v>6</v>
       </c>
@@ -2349,11 +2367,11 @@
       <c r="H60" s="8">
         <v>0.1</v>
       </c>
-      <c r="I60" s="39"/>
+      <c r="I60" s="32"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="37"/>
-      <c r="B61" s="32"/>
+      <c r="A61" s="35"/>
+      <c r="B61" s="33"/>
       <c r="C61" s="3" t="s">
         <v>9</v>
       </c>
@@ -2369,11 +2387,11 @@
       <c r="H61" s="8">
         <v>0.1</v>
       </c>
-      <c r="I61" s="39"/>
+      <c r="I61" s="32"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="37"/>
-      <c r="B62" s="32"/>
+      <c r="A62" s="35"/>
+      <c r="B62" s="33"/>
       <c r="C62" s="3" t="s">
         <v>10</v>
       </c>
@@ -2389,11 +2407,11 @@
       <c r="H62" s="8">
         <v>0.1</v>
       </c>
-      <c r="I62" s="39"/>
+      <c r="I62" s="32"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="37"/>
-      <c r="B63" s="32"/>
+      <c r="A63" s="35"/>
+      <c r="B63" s="33"/>
       <c r="C63" s="3" t="s">
         <v>56</v>
       </c>
@@ -2409,11 +2427,11 @@
       <c r="H63" s="8">
         <v>0.05</v>
       </c>
-      <c r="I63" s="39"/>
+      <c r="I63" s="32"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="37"/>
-      <c r="B64" s="32"/>
+      <c r="A64" s="35"/>
+      <c r="B64" s="33"/>
       <c r="C64" s="9" t="s">
         <v>3</v>
       </c>
@@ -2429,11 +2447,11 @@
       <c r="H64" s="8">
         <v>0.05</v>
       </c>
-      <c r="I64" s="39"/>
+      <c r="I64" s="32"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="37"/>
-      <c r="B65" s="32"/>
+      <c r="A65" s="35"/>
+      <c r="B65" s="33"/>
       <c r="C65" s="2" t="s">
         <v>4</v>
       </c>
@@ -2449,11 +2467,11 @@
       <c r="H65" s="8">
         <v>0.05</v>
       </c>
-      <c r="I65" s="39"/>
+      <c r="I65" s="32"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="37"/>
-      <c r="B66" s="32"/>
+      <c r="A66" s="35"/>
+      <c r="B66" s="33"/>
       <c r="C66" s="2" t="s">
         <v>5</v>
       </c>
@@ -2469,11 +2487,11 @@
       <c r="H66" s="8">
         <v>0.05</v>
       </c>
-      <c r="I66" s="39"/>
+      <c r="I66" s="32"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="37"/>
-      <c r="B67" s="32"/>
+      <c r="A67" s="35"/>
+      <c r="B67" s="33"/>
       <c r="C67" s="2" t="s">
         <v>7</v>
       </c>
@@ -2489,11 +2507,11 @@
       <c r="H67" s="8">
         <v>0.1</v>
       </c>
-      <c r="I67" s="39"/>
+      <c r="I67" s="32"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="37"/>
-      <c r="B68" s="32"/>
+      <c r="A68" s="35"/>
+      <c r="B68" s="33"/>
       <c r="C68" s="2" t="s">
         <v>12</v>
       </c>
@@ -2509,11 +2527,11 @@
       <c r="H68" s="8">
         <v>0.1</v>
       </c>
-      <c r="I68" s="39"/>
+      <c r="I68" s="32"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="37"/>
-      <c r="B69" s="32"/>
+      <c r="A69" s="35"/>
+      <c r="B69" s="33"/>
       <c r="C69" s="2" t="s">
         <v>13</v>
       </c>
@@ -2529,11 +2547,11 @@
       <c r="H69" s="8">
         <v>0.05</v>
       </c>
-      <c r="I69" s="39"/>
+      <c r="I69" s="32"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="37"/>
-      <c r="B70" s="32"/>
+      <c r="A70" s="35"/>
+      <c r="B70" s="33"/>
       <c r="C70" s="6" t="s">
         <v>38</v>
       </c>
@@ -2549,11 +2567,11 @@
       <c r="H70" s="8">
         <v>0.05</v>
       </c>
-      <c r="I70" s="39"/>
+      <c r="I70" s="32"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="37"/>
-      <c r="B71" s="32"/>
+      <c r="A71" s="35"/>
+      <c r="B71" s="33"/>
       <c r="C71" s="6" t="s">
         <v>39</v>
       </c>
@@ -2569,7 +2587,7 @@
       <c r="H71" s="8">
         <v>0.05</v>
       </c>
-      <c r="I71" s="39"/>
+      <c r="I71" s="32"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
@@ -2608,6 +2626,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B22:B42"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B47:B54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B12:B21"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="B58:B71"/>
+    <mergeCell ref="A58:A71"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="A22:A42"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A47:A54"/>
     <mergeCell ref="H2:H11"/>
     <mergeCell ref="H12:H21"/>
     <mergeCell ref="F2:F11"/>
@@ -2618,22 +2652,6 @@
     <mergeCell ref="I22:I42"/>
     <mergeCell ref="I43:I46"/>
     <mergeCell ref="I47:I54"/>
-    <mergeCell ref="B58:B71"/>
-    <mergeCell ref="A58:A71"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A12:A21"/>
-    <mergeCell ref="A22:A42"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A47:A54"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B22:B42"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B47:B54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B12:B21"/>
-    <mergeCell ref="B2:B11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C36" r:id="rId1" display="http://umbrella/jqgrid/jqgrid/newpage/1/container/test_history_15677/oper/information/db/xt/table/testcase/element/15677/parent/5002157/ver/78043"/>
@@ -2646,10 +2664,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,47 +2675,72 @@
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" customWidth="1"/>
     <col min="3" max="3" width="4.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
       <c r="D1" s="40" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="40"/>
       <c r="H1" s="40"/>
       <c r="I1" s="40"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="40"/>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="E2" s="40"/>
       <c r="F2" s="40" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="G2" s="40"/>
       <c r="H2" s="40" t="s">
         <v>71</v>
       </c>
       <c r="I2" s="40"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" s="40"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -2719,10 +2762,28 @@
       <c r="I3" s="27" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>110</v>
+      <c r="J3" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>82</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -2731,22 +2792,28 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2754,22 +2821,28 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2777,22 +2850,28 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -2800,22 +2879,28 @@
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
@@ -2823,22 +2908,28 @@
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
       <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
@@ -2846,72 +2937,102 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
       <c r="B10" s="3" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="C10" s="26">
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
       <c r="B11" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="26">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+        <v>97</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
@@ -2919,26 +3040,32 @@
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+        <v>106</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
@@ -2946,26 +3073,32 @@
         <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>75</v>
+        <v>121</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>75</v>
+        <v>121</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+        <v>117</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="33"/>
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
@@ -2973,26 +3106,32 @@
         <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+        <v>105</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
@@ -3000,26 +3139,32 @@
         <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+        <v>127</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -3027,26 +3172,32 @@
         <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+        <v>98</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -3054,26 +3205,32 @@
         <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+        <v>112</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
       <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
@@ -3081,26 +3238,32 @@
         <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="H18" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+        <v>125</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
@@ -3108,53 +3271,77 @@
         <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+        <v>116</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
       <c r="B20" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="26">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+        <v>111</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
       <c r="B21" s="6" t="s">
         <v>38</v>
       </c>
@@ -3162,26 +3349,32 @@
         <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+        <v>108</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
       <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
@@ -3189,26 +3382,32 @@
         <v>6</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="I22" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+        <v>97</v>
+      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
       <c r="B23" s="6" t="s">
         <v>40</v>
       </c>
@@ -3216,18 +3415,24 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
       <c r="B24" s="2" t="s">
         <v>14</v>
       </c>
@@ -3235,207 +3440,213 @@
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="28"/>
       <c r="D27" s="27" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="38" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="C28" s="26">
         <v>2</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="38"/>
       <c r="B29" s="2" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="C29" s="26">
         <v>2</v>
       </c>
       <c r="D29" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="38"/>
+      <c r="B30" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="C30" s="26">
         <v>2</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="38"/>
       <c r="B31" s="2" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="C31" s="26">
         <v>2</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="38" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>19</v>
+        <v>130</v>
       </c>
       <c r="C32" s="26">
         <v>1</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="2" t="s">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C33" s="26">
         <v>1</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="2" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="C34" s="26">
         <v>1</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="2" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="C35" s="26">
         <v>1</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
+      <c r="A36" s="38"/>
       <c r="B36" s="2" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="C36" s="26">
         <v>1</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
+      <c r="A37" s="38"/>
       <c r="B37" s="2" t="s">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="C37" s="26">
         <v>1</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="38"/>
       <c r="B38" s="2" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="C38" s="26">
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
+      <c r="A39" s="38"/>
       <c r="B39" s="2" t="s">
-        <v>26</v>
+        <v>129</v>
       </c>
       <c r="C39" s="26">
         <v>1</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="33" t="s">
         <v>57</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -3445,12 +3656,12 @@
         <v>1</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="A41" s="33"/>
       <c r="B41" s="3" t="s">
         <v>8</v>
       </c>
@@ -3458,12 +3669,12 @@
         <v>1</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
+      <c r="A42" s="33"/>
       <c r="B42" s="3" t="s">
         <v>6</v>
       </c>
@@ -3471,12 +3682,12 @@
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="3" t="s">
         <v>9</v>
       </c>
@@ -3484,12 +3695,12 @@
         <v>1</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
+      <c r="A44" s="33"/>
       <c r="B44" s="3" t="s">
         <v>10</v>
       </c>
@@ -3497,12 +3708,12 @@
         <v>1</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+      <c r="A45" s="33"/>
       <c r="B45" s="3" t="s">
         <v>56</v>
       </c>
@@ -3510,12 +3721,12 @@
         <v>1</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
+      <c r="A46" s="33"/>
       <c r="B46" s="9" t="s">
         <v>3</v>
       </c>
@@ -3523,12 +3734,12 @@
         <v>1</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
+      <c r="A47" s="33"/>
       <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
@@ -3536,12 +3747,12 @@
         <v>1</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
+      <c r="A48" s="33"/>
       <c r="B48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3549,12 +3760,12 @@
         <v>1</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="2" t="s">
         <v>7</v>
       </c>
@@ -3562,12 +3773,12 @@
         <v>1</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
+      <c r="A50" s="33"/>
       <c r="B50" s="2" t="s">
         <v>12</v>
       </c>
@@ -3575,12 +3786,12 @@
         <v>1</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+      <c r="A51" s="33"/>
       <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
@@ -3588,12 +3799,12 @@
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
+      <c r="A52" s="33"/>
       <c r="B52" s="6" t="s">
         <v>38</v>
       </c>
@@ -3601,12 +3812,12 @@
         <v>1</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
+      <c r="A53" s="33"/>
       <c r="B53" s="6" t="s">
         <v>39</v>
       </c>
@@ -3614,18 +3825,22 @@
         <v>1</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E53" s="2"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C55" s="22">
         <f>SUM(C4:C53)</f>
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
     <mergeCell ref="A40:A53"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
@@ -3661,13 +3876,13 @@
   <sheetData>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3675,13 +3890,13 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="43"/>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>